<commit_message>
Verificando se script "analise estat..." está okay
</commit_message>
<xml_diff>
--- a/Projeto PIBITI/Resultados Analise/medias finais/A009_PALMAS.xlsx
+++ b/Projeto PIBITI/Resultados Analise/medias finais/A009_PALMAS.xlsx
@@ -116,10 +116,10 @@
     <t>Least Squares</t>
   </si>
   <si>
-    <t>Wed, 01 Sep 2021</t>
-  </si>
-  <si>
-    <t>14:11:03</t>
+    <t>Wed, 29 Sep 2021</t>
+  </si>
+  <si>
+    <t>13:44:38</t>
   </si>
   <si>
     <t>365</t>
@@ -203,7 +203,7 @@
     <t>R</t>
   </si>
   <si>
-    <t>14:11:08</t>
+    <t>13:44:50</t>
   </si>
 </sst>
 </file>

</xml_diff>